<commit_message>
Updated admin functions for invitations. Created users collection in firestore. Added admin function to get user data from registrations.
</commit_message>
<xml_diff>
--- a/public/data/invitees_test.xlsx
+++ b/public/data/invitees_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tok\Code\runners-hub\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tok\Code\runners-hub\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA431183-E066-49E9-9F20-36F98C26E899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6D81BA-A0AE-4E93-8F88-361E294B481D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{AEE88481-E58B-4B04-B9A8-71BD23EC5F19}"/>
   </bookViews>
@@ -47,17 +47,17 @@
     <t>name</t>
   </si>
   <si>
-    <t>torgeir.kruke@gmail.com</t>
+    <t>Kjetil</t>
   </si>
   <si>
-    <t>Torgeir</t>
+    <t>gotvassli@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,14 +69,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -97,17 +89,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,7 +432,7 @@
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,11 +449,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -648,9 +637,6 @@
       <c r="B47" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{2D0FBDD6-CFE4-4501-8F5D-12164BAB0C29}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K0000FF Klassifisering: Intern informasjon&amp;1#_x000D_</oddHeader>

</xml_diff>